<commit_message>
updated commodities and sets
</commit_message>
<xml_diff>
--- a/Data/sets.xlsx
+++ b/Data/sets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\GitHub\STraM_ntnu_development\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1286D3D6-CC95-4AC3-841C-6513F4497C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8EDCB7-3071-4B6D-93C0-42295096A559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modes" sheetId="5" r:id="rId1"/>
@@ -63,12 +63,6 @@
     <t>Break bulk</t>
   </si>
   <si>
-    <t>Neo bulk (fast)</t>
-  </si>
-  <si>
-    <t>Neo bulk (slow)</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -151,6 +145,12 @@
   </si>
   <si>
     <t>Lifetime</t>
+  </si>
+  <si>
+    <t>Break bulk (fast)</t>
+  </si>
+  <si>
+    <t>Break bulk (slow)</t>
   </si>
 </sst>
 </file>
@@ -490,62 +490,62 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -560,219 +560,219 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D3DC6D-0270-48DE-95C0-A9C75EDC81AD}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -784,20 +784,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -806,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -817,7 +817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -828,7 +828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -836,10 +836,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -847,40 +847,40 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -897,25 +897,25 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -926,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -937,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -948,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -959,7 +959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -983,29 +983,29 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="90.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>